<commit_message>
added Yes|No delegates, labels for Dropbox delegates and OpenFile delegates
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB2B183-8315-4B10-A6D4-40E8644342A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D522D068-D729-42AC-8227-3EC9538F3B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
   <si>
     <t>Путь</t>
   </si>
@@ -322,9 +322,6 @@
     <t>numerical</t>
   </si>
   <si>
-    <t>cases=[0, 1]</t>
-  </si>
-  <si>
     <t>cases=[1, 2, 3]</t>
   </si>
   <si>
@@ -350,6 +347,12 @@
   </si>
   <si>
     <t>minimisation</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>cases=[0, 1]; labels=['Эксперимент', 'SIMTRA']</t>
   </si>
 </sst>
 </file>
@@ -720,15 +723,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1796875" customWidth="1"/>
     <col min="7" max="7" width="111.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -813,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
         <v>97</v>
@@ -836,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
         <v>97</v>
@@ -970,8 +973,8 @@
       <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="D11">
-        <v>1</v>
+      <c r="D11" t="s">
+        <v>109</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -993,8 +996,8 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12">
-        <v>1</v>
+      <c r="D12" t="s">
+        <v>109</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -1172,10 +1175,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1195,10 +1198,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21">
         <v>0.01</v>
@@ -1215,10 +1218,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22">
         <v>0.01</v>
@@ -1396,7 +1399,7 @@
         <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G30" t="s">
         <v>87</v>
@@ -1419,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G31" t="s">
         <v>87</v>
@@ -1442,7 +1445,7 @@
         <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G32" t="s">
         <v>87</v>
@@ -1462,10 +1465,10 @@
         <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G33" t="s">
         <v>88</v>
@@ -1488,7 +1491,7 @@
         <v>59</v>
       </c>
       <c r="F34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G34" t="s">
         <v>60</v>
@@ -1511,7 +1514,7 @@
         <v>59</v>
       </c>
       <c r="F35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
         <v>63</v>
@@ -1534,7 +1537,7 @@
         <v>59</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G36" t="s">
         <v>89</v>
@@ -1557,7 +1560,7 @@
         <v>68</v>
       </c>
       <c r="F37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G37" t="s">
         <v>69</v>
@@ -1580,7 +1583,7 @@
         <v>68</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G38" t="s">
         <v>72</v>
@@ -1603,7 +1606,7 @@
         <v>68</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G39" t="s">
         <v>90</v>
@@ -1626,7 +1629,7 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G40" t="s">
         <v>77</v>
@@ -1649,7 +1652,7 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G41" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
added units, costul fixed
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D522D068-D729-42AC-8227-3EC9538F3B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32427B2F-278E-46F5-8342-1649E53569C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
   <si>
     <t>Путь</t>
   </si>
@@ -175,15 +175,6 @@
     <t>deposition_res_y</t>
   </si>
   <si>
-    <t>Границы R</t>
-  </si>
-  <si>
-    <t>Границы k</t>
-  </si>
-  <si>
-    <t>Границы числа поворотов</t>
-  </si>
-  <si>
     <t>Алгоритм минимизации</t>
   </si>
   <si>
@@ -353,6 +344,39 @@
   </si>
   <si>
     <t>cases=[0, 1]; labels=['Эксперимент', 'SIMTRA']</t>
+  </si>
+  <si>
+    <t>нм/мин</t>
+  </si>
+  <si>
+    <t>мм</t>
+  </si>
+  <si>
+    <t>1/мм</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Нижняя граница R</t>
+  </si>
+  <si>
+    <t>Верхняя граница R</t>
+  </si>
+  <si>
+    <t>Нижняя граница k</t>
+  </si>
+  <si>
+    <t>Нижняя граница NR</t>
+  </si>
+  <si>
+    <t>Верхняя граница k</t>
+  </si>
+  <si>
+    <t>Верхняя граница NR</t>
+  </si>
+  <si>
+    <t>обороты</t>
   </si>
 </sst>
 </file>
@@ -721,42 +745,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="111.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="111.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
       <c r="B1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -769,17 +799,17 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
       <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -793,16 +823,19 @@
         <v>4.46</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -815,17 +848,17 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>110</v>
-      </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -838,17 +871,17 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
       <c r="F5" t="s">
         <v>97</v>
       </c>
       <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -862,16 +895,19 @@
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -885,16 +921,19 @@
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -908,16 +947,19 @@
         <v>0.05</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -931,16 +973,19 @@
         <v>0.05</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -953,17 +998,17 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s">
-        <v>98</v>
-      </c>
       <c r="G10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -974,19 +1019,19 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
-        <v>98</v>
-      </c>
       <c r="G11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -997,19 +1042,19 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>98</v>
-      </c>
       <c r="G12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1020,19 +1065,22 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1045,17 +1093,17 @@
       <c r="D14">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" t="s">
-        <v>99</v>
-      </c>
       <c r="G14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1069,16 +1117,19 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1092,16 +1143,19 @@
         <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F16" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1115,16 +1169,19 @@
         <v>290</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1138,16 +1195,19 @@
         <v>290</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1161,79 +1221,88 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
         <v>102</v>
-      </c>
-      <c r="C20" t="s">
-        <v>105</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
         <v>103</v>
-      </c>
-      <c r="C21" t="s">
-        <v>106</v>
       </c>
       <c r="D21">
         <v>0.01</v>
       </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
       <c r="F21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" t="s">
         <v>104</v>
-      </c>
-      <c r="C22" t="s">
-        <v>107</v>
       </c>
       <c r="D22">
         <v>0.01</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1247,415 +1316,451 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G23" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D25">
         <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>6</v>
-      </c>
       <c r="F26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D27">
         <v>50</v>
       </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
       <c r="F27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D29">
         <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="F29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D30">
         <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="G30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="F32" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="G32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
         <v>57</v>
       </c>
-      <c r="C34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34">
-        <v>0.05</v>
-      </c>
-      <c r="E34" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" t="s">
-        <v>108</v>
-      </c>
-      <c r="G34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D35">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="F35" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D36">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D38">
         <v>0.01</v>
       </c>
-      <c r="E38" t="s">
-        <v>68</v>
-      </c>
       <c r="F38" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="G38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="G39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>26</v>
       </c>
-      <c r="F40" t="s">
-        <v>108</v>
-      </c>
       <c r="G40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="H40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
-        <v>6</v>
-      </c>
       <c r="F41" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>80</v>
+        <v>105</v>
+      </c>
+      <c r="H41" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug with multiprocessing fixed, but it still running very uneffecient
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32427B2F-278E-46F5-8342-1649E53569C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C9D46D-7D24-446B-A735-129141DF1DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>depz.txt</t>
   </si>
   <si>
-    <t>path to dep profile</t>
-  </si>
-  <si>
     <t>Скорость осаждения</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>+float</t>
   </si>
   <si>
-    <t>thickness [nm] per minute</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -377,6 +371,12 @@
   </si>
   <si>
     <t>обороты</t>
+  </si>
+  <si>
+    <t>Скорость роста плёнки [нм/мин]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Путь к файлу с результатами расчёта SIMTRA.  </t>
   </si>
 </sst>
 </file>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,10 +803,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -814,25 +814,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="D3">
         <v>4.46</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -840,22 +840,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -863,22 +863,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -886,25 +886,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -912,25 +912,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -938,25 +938,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>0.05</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -964,25 +964,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>0.05</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -990,22 +990,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1013,22 +1013,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1036,22 +1036,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1059,25 +1059,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1085,22 +1085,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1108,25 +1108,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1134,25 +1134,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1160,25 +1160,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>290</v>
       </c>
       <c r="E17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1186,25 +1186,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>290</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1212,25 +1212,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1238,25 +1238,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1264,19 +1264,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D21">
         <v>0.01</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1284,22 +1284,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22">
         <v>0.01</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1307,25 +1307,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1333,25 +1333,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1359,25 +1359,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D25">
         <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1385,19 +1385,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1405,19 +1405,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27">
         <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1425,22 +1425,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1448,22 +1448,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D29">
         <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1471,25 +1471,25 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1497,22 +1497,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D31">
         <v>4.0999999999999996</v>
       </c>
       <c r="F31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1520,25 +1520,25 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1546,22 +1546,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
         <v>51</v>
       </c>
-      <c r="C33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
       <c r="F33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1569,25 +1569,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" t="s">
         <v>54</v>
       </c>
-      <c r="C34" t="s">
+      <c r="G34" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" t="s">
         <v>55</v>
-      </c>
-      <c r="D34">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G34" t="s">
-        <v>105</v>
-      </c>
-      <c r="H34" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1595,25 +1595,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" t="s">
         <v>58</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35">
-        <v>5</v>
-      </c>
-      <c r="E35" t="s">
-        <v>111</v>
-      </c>
-      <c r="F35" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" t="s">
-        <v>105</v>
-      </c>
-      <c r="H35" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1621,25 +1621,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -1647,25 +1647,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -1673,22 +1673,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D38">
         <v>0.01</v>
       </c>
       <c r="F38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -1696,25 +1696,25 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -1722,22 +1722,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1745,22 +1745,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
depliney input file format changed, joblib and multiprocesing versions of deposition func was deleted, now only ray version is available
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C9D46D-7D24-446B-A735-129141DF1DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6467F1F-2EDB-4130-80C4-4D25C0977652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
-  <si>
-    <t>Путь</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="131">
   <si>
     <t>filename</t>
   </si>
@@ -46,12 +43,6 @@
     <t>Choose source of get thickness data 1 - seimtra, 0 - experiment</t>
   </si>
   <si>
-    <t>val</t>
-  </si>
-  <si>
-    <t>1, 2, 3 - magnetron position</t>
-  </si>
-  <si>
     <t>Длина подложки</t>
   </si>
   <si>
@@ -307,9 +298,6 @@
     <t>numerical</t>
   </si>
   <si>
-    <t>cases=[1, 2, 3]</t>
-  </si>
-  <si>
     <t>cases=['NM_custom', 'NM', 'Powell']</t>
   </si>
   <si>
@@ -337,9 +325,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>cases=[0, 1]; labels=['Эксперимент', 'SIMTRA']</t>
-  </si>
-  <si>
     <t>нм/мин</t>
   </si>
   <si>
@@ -377,6 +362,57 @@
   </si>
   <si>
     <t xml:space="preserve">Путь к файлу с результатами расчёта SIMTRA.  </t>
+  </si>
+  <si>
+    <t>Минимальный радиус</t>
+  </si>
+  <si>
+    <t>Максимальный радиус</t>
+  </si>
+  <si>
+    <t>Минимальный радиус, на котором могут находиться точки подложки. Может определяться геометрическими размерами оси вращения и навесными устройствами. Исходя из значения этого параметра программа определяет возможный диапазон изменения радиуса орбиты планетарной шестерни.</t>
+  </si>
+  <si>
+    <t>Максимальный радиус, на котором могут находиться точки подложки. Может определяться геометрическими размерами оси вращения и навесными устройствами. Исходя из значения этого параметра программа определяет возможный диапазон изменения радиуса орбиты планетарной шестерни.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ширина области напыления </t>
+  </si>
+  <si>
+    <t>Высота области напыления</t>
+  </si>
+  <si>
+    <t>Размеры области напыления о оси х</t>
+  </si>
+  <si>
+    <t>Размеры области напыления о оси у</t>
+  </si>
+  <si>
+    <t>Результаты расчёта SIMTRA</t>
+  </si>
+  <si>
+    <t>fname_sim</t>
+  </si>
+  <si>
+    <t>cases=['Experiment', 'SIMTRA']</t>
+  </si>
+  <si>
+    <t>Позиция магнетрона х</t>
+  </si>
+  <si>
+    <t>Позиция магнетрона у</t>
+  </si>
+  <si>
+    <t>magnetron_x</t>
+  </si>
+  <si>
+    <t>magnetron_y</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Experiment</t>
   </si>
 </sst>
 </file>
@@ -438,11 +474,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -745,16 +782,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
     <col min="6" max="6" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1796875" customWidth="1"/>
     <col min="8" max="8" width="111.08984375" bestFit="1" customWidth="1"/>
@@ -791,22 +829,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -814,25 +852,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
       <c r="D3">
         <v>4.46</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -840,22 +878,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -863,22 +901,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
+        <v>127</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-105.8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -886,25 +924,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
+        <v>128</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -912,25 +947,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -938,25 +973,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -964,25 +999,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>0.05</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -990,22 +1025,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.05</v>
+      </c>
+      <c r="E10" t="s">
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1013,22 +1051,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1036,22 +1074,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1059,25 +1097,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>109</v>
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1085,22 +1120,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1108,25 +1146,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D15">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>107</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1134,25 +1169,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D16">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1160,25 +1195,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17">
-        <v>290</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1186,25 +1221,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D18">
         <v>290</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1212,25 +1247,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>290</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H19" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1238,25 +1273,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1264,19 +1299,25 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D21">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>102</v>
       </c>
       <c r="F21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1284,22 +1325,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D22">
         <v>0.01</v>
       </c>
-      <c r="E22" t="s">
-        <v>116</v>
-      </c>
       <c r="F22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1307,25 +1345,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1333,25 +1368,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1359,25 +1394,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D25">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1385,19 +1420,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="H26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1405,19 +1446,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1425,22 +1466,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>116</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1448,22 +1486,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D29">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1471,25 +1509,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D30">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1497,22 +1532,25 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D31">
-        <v>4.0999999999999996</v>
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1520,25 +1558,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>116</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1546,22 +1581,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" t="s">
-        <v>51</v>
+        <v>85</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>111</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="G33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1569,25 +1607,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>109</v>
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="G34" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H34" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1595,25 +1630,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D35">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G35" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H35" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1621,25 +1656,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D36">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H36" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -1647,25 +1682,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F37" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H37" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -1673,22 +1708,25 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D38">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>102</v>
       </c>
       <c r="F38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H38" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -1696,25 +1734,22 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>116</v>
+        <v>0.01</v>
       </c>
       <c r="F39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H39" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -1722,22 +1757,25 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>111</v>
       </c>
       <c r="F40" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="G40" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H40" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1745,22 +1783,45 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H41" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read source from file reorganized
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6467F1F-2EDB-4130-80C4-4D25C0977652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5263987B-F75C-45AE-A703-EBF660359648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="130">
   <si>
     <t>filename</t>
   </si>
@@ -145,21 +145,6 @@
     <t>deposition_len_y</t>
   </si>
   <si>
-    <t>Разрешение по х источника</t>
-  </si>
-  <si>
-    <t>deposition_res_x</t>
-  </si>
-  <si>
-    <t>1/mm</t>
-  </si>
-  <si>
-    <t>Разрешение по у источника</t>
-  </si>
-  <si>
-    <t>deposition_res_y</t>
-  </si>
-  <si>
     <t>Алгоритм минимизации</t>
   </si>
   <si>
@@ -413,6 +398,18 @@
   </si>
   <si>
     <t>Experiment</t>
+  </si>
+  <si>
+    <t>Экспериментальный профиль</t>
+  </si>
+  <si>
+    <t>fname_exp</t>
+  </si>
+  <si>
+    <t>depliney.txt</t>
+  </si>
+  <si>
+    <t>Путь к файлу с экспериментальным профилем напыления.</t>
   </si>
 </sst>
 </file>
@@ -782,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -841,10 +838,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -852,25 +849,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4.46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>101</v>
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -878,22 +872,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>130</v>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4.46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -901,22 +898,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-105.8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>102</v>
-      </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -924,22 +921,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>-105.8</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -947,25 +944,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>100</v>
+        <v>123</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -973,25 +967,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -999,25 +993,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1025,25 +1019,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>0.05</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1051,22 +1045,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.05</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1074,22 +1071,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1097,22 +1094,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1120,25 +1117,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>104</v>
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1146,22 +1140,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1169,25 +1166,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1195,25 +1189,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1221,25 +1215,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18">
-        <v>290</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H18" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1247,25 +1241,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>290</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F19" t="s">
         <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1273,25 +1267,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>290</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1299,22 +1293,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H21" t="s">
         <v>37</v>
@@ -1325,10 +1319,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D22">
         <v>0.01</v>
@@ -1337,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1345,22 +1339,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D23">
         <v>0.01</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1368,25 +1362,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1394,22 +1388,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F25" t="s">
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H25" t="s">
         <v>37</v>
@@ -1420,25 +1414,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D26">
-        <v>65</v>
-      </c>
-      <c r="E26" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1446,19 +1434,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1466,19 +1454,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1486,22 +1477,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1509,22 +1500,25 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
         <v>78</v>
       </c>
       <c r="D30">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>94</v>
+      </c>
+      <c r="H30" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1532,25 +1526,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D31">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>102</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F31" t="s">
         <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1558,22 +1549,25 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D32">
-        <v>4.0999999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1581,25 +1575,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>111</v>
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="G33" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1607,22 +1598,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" t="s">
         <v>46</v>
       </c>
-      <c r="C34" t="s">
+      <c r="G34" t="s">
+        <v>94</v>
+      </c>
+      <c r="H34" t="s">
         <v>47</v>
-      </c>
-      <c r="D34" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G34" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1630,25 +1624,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
         <v>49</v>
-      </c>
-      <c r="C35" t="s">
-        <v>50</v>
       </c>
       <c r="D35">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F35" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1656,25 +1650,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F36" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H36" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -1682,25 +1676,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" t="s">
+        <v>94</v>
+      </c>
+      <c r="H37" t="s">
         <v>56</v>
-      </c>
-      <c r="C37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37">
-        <v>15</v>
-      </c>
-      <c r="E37" t="s">
-        <v>104</v>
-      </c>
-      <c r="F37" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -1708,25 +1702,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
         <v>58</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38">
+        <v>0.01</v>
+      </c>
+      <c r="F38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" t="s">
+        <v>94</v>
+      </c>
+      <c r="H38" t="s">
         <v>59</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>102</v>
-      </c>
-      <c r="F38" t="s">
-        <v>60</v>
-      </c>
-      <c r="G38" t="s">
-        <v>99</v>
-      </c>
-      <c r="H38" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -1734,22 +1725,25 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>106</v>
       </c>
       <c r="F39" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H39" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -1757,25 +1751,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="G40" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H40" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1783,45 +1774,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="F42" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exception hooks and log file was added
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5263987B-F75C-45AE-A703-EBF660359648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A042D-67D0-4E79-9BB7-618B59453ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
open file delegate was changed, icon for open file dialog was added - ura!
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A042D-67D0-4E79-9BB7-618B59453ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757805C5-AE75-4E45-900D-456B8629F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="146">
   <si>
     <t>filename</t>
   </si>
@@ -410,6 +410,54 @@
   </si>
   <si>
     <t>Путь к файлу с экспериментальным профилем напыления.</t>
+  </si>
+  <si>
+    <t>Тип вращения</t>
+  </si>
+  <si>
+    <t>rotation_type</t>
+  </si>
+  <si>
+    <t>Planet</t>
+  </si>
+  <si>
+    <t>cases=['Planet', 'Solar']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тип вращения подложкодержателя. </t>
+  </si>
+  <si>
+    <t>substrate_shape</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>Форма подложки</t>
+  </si>
+  <si>
+    <t>cases=['Circle', 'Rectangle']</t>
+  </si>
+  <si>
+    <t>Радиус подложки</t>
+  </si>
+  <si>
+    <t>substrate_radius</t>
+  </si>
+  <si>
+    <t>Макс. угловая скорость солнца</t>
+  </si>
+  <si>
+    <t>Макс. угловая скорость планеты</t>
+  </si>
+  <si>
+    <t>omega_s_max</t>
+  </si>
+  <si>
+    <t>omega_p_max</t>
+  </si>
+  <si>
+    <t>оборотов/мин</t>
   </si>
 </sst>
 </file>
@@ -779,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -790,6 +838,7 @@
     <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1796875" customWidth="1"/>
     <col min="8" max="8" width="111.08984375" bestFit="1" customWidth="1"/>
@@ -967,25 +1016,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
+        <v>135</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="G8" t="s">
         <v>84</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -993,13 +1036,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
+        <v>140</v>
+      </c>
+      <c r="D9" s="2">
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>97</v>
@@ -1009,9 +1052,6 @@
       </c>
       <c r="G9" t="s">
         <v>84</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1019,25 +1059,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1045,25 +1085,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1071,22 +1111,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.05</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1094,22 +1137,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>95</v>
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>0.05</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1117,22 +1163,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
         <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1140,25 +1186,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>99</v>
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>95</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1166,22 +1209,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1189,25 +1232,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F17" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H17" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1215,25 +1258,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18">
-        <v>145</v>
-      </c>
-      <c r="E18" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1241,13 +1281,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D19">
-        <v>290</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>97</v>
@@ -1259,7 +1299,7 @@
         <v>84</v>
       </c>
       <c r="H19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1267,13 +1307,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20">
-        <v>290</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
         <v>97</v>
@@ -1285,7 +1325,7 @@
         <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1293,13 +1333,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>290</v>
       </c>
       <c r="E21" t="s">
         <v>97</v>
@@ -1311,7 +1351,7 @@
         <v>84</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1319,19 +1359,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D22">
-        <v>0.01</v>
+        <v>290</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
       </c>
       <c r="G22" t="s">
         <v>84</v>
+      </c>
+      <c r="H22" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1339,22 +1385,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
       <c r="G23" t="s">
         <v>84</v>
+      </c>
+      <c r="H23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1362,25 +1411,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D24">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>97</v>
+        <v>0.01</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
       </c>
       <c r="G24" t="s">
         <v>84</v>
-      </c>
-      <c r="H24" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1388,25 +1431,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="D25">
-        <v>65</v>
+        <v>0.01</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
         <v>4</v>
       </c>
       <c r="G25" t="s">
         <v>84</v>
-      </c>
-      <c r="H25" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1414,19 +1454,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
       </c>
       <c r="G26" t="s">
         <v>84</v>
+      </c>
+      <c r="H26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1434,19 +1480,25 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27">
-        <v>50</v>
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
       <c r="G27" t="s">
         <v>84</v>
+      </c>
+      <c r="H27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1454,16 +1506,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28">
         <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>106</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
@@ -1477,16 +1526,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D29">
-        <v>100</v>
-      </c>
-      <c r="E29" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -1500,25 +1546,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D30">
-        <v>35</v>
+        <v>0.01</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>94</v>
-      </c>
-      <c r="H30" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1526,22 +1569,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D31">
-        <v>4.0999999999999996</v>
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
       </c>
       <c r="F31" t="s">
         <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
-      </c>
-      <c r="H31" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1549,25 +1592,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>94</v>
-      </c>
-      <c r="H32" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1575,22 +1615,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" t="s">
-        <v>43</v>
+        <v>144</v>
+      </c>
+      <c r="D33">
+        <v>100</v>
+      </c>
+      <c r="E33" t="s">
+        <v>145</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
-      </c>
-      <c r="H33" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1598,25 +1638,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="G34" t="s">
         <v>94</v>
       </c>
       <c r="H34" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1624,25 +1664,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D35">
-        <v>5</v>
-      </c>
-      <c r="E35" t="s">
-        <v>99</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="G35" t="s">
         <v>94</v>
       </c>
       <c r="H35" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1650,25 +1687,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D36">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="G36" t="s">
         <v>94</v>
       </c>
       <c r="H36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -1676,25 +1713,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>97</v>
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
         <v>94</v>
       </c>
       <c r="H37" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -1702,22 +1736,25 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D38">
-        <v>0.01</v>
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>99</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G38" t="s">
         <v>94</v>
       </c>
       <c r="H38" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -1725,25 +1762,25 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F39" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G39" t="s">
         <v>94</v>
       </c>
       <c r="H39" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -1751,22 +1788,25 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>99</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G40" t="s">
         <v>94</v>
       </c>
       <c r="H40" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1774,22 +1814,143 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>97</v>
       </c>
       <c r="F41" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="G41" t="s">
         <v>94</v>
       </c>
       <c r="H41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42">
+        <v>0.01</v>
+      </c>
+      <c r="F42" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" t="s">
+        <v>94</v>
+      </c>
+      <c r="H43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" t="s">
+        <v>94</v>
+      </c>
+      <c r="H45" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+      <c r="F46" t="s">
+        <v>133</v>
+      </c>
+      <c r="G46" t="s">
+        <v>84</v>
+      </c>
+      <c r="H46" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bag with Enter shortcut
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757805C5-AE75-4E45-900D-456B8629F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E1985E-68AB-41E6-B859-E18C155E9CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,22 +875,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="G2" t="s">
         <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -898,13 +898,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>84</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -921,25 +921,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>4.46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>96</v>
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -947,22 +944,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-105.8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
         <v>84</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -970,13 +967,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D6" s="2">
-        <v>-105.8</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>97</v>
@@ -993,22 +990,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4.46</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>84</v>
+      </c>
+      <c r="H7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1016,19 +1016,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>136</v>
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>290</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
         <v>84</v>
+      </c>
+      <c r="H8" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1036,13 +1042,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="2">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>290</v>
       </c>
       <c r="E9" t="s">
         <v>97</v>
@@ -1052,6 +1058,9 @@
       </c>
       <c r="G9" t="s">
         <v>84</v>
+      </c>
+      <c r="H9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1059,13 +1068,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>97</v>
@@ -1077,7 +1086,7 @@
         <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1085,13 +1094,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
         <v>97</v>
@@ -1103,7 +1112,7 @@
         <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1111,25 +1120,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12">
-        <v>0.05</v>
-      </c>
-      <c r="E12" t="s">
-        <v>98</v>
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1137,25 +1143,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <v>0.05</v>
-      </c>
-      <c r="E13" t="s">
-        <v>98</v>
+        <v>135</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1163,22 +1163,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="D14" s="2">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1186,22 +1186,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>95</v>
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1209,22 +1212,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>95</v>
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1232,25 +1238,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1258,22 +1264,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1281,25 +1284,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>0.01</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
         <v>4</v>
       </c>
       <c r="G19" t="s">
         <v>84</v>
-      </c>
-      <c r="H19" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1307,13 +1307,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D20">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
         <v>97</v>
@@ -1325,7 +1325,7 @@
         <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1333,13 +1333,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="D21">
-        <v>290</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
         <v>97</v>
@@ -1351,7 +1351,7 @@
         <v>84</v>
       </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1359,25 +1359,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="D22">
-        <v>290</v>
-      </c>
-      <c r="E22" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
       </c>
       <c r="G22" t="s">
         <v>84</v>
-      </c>
-      <c r="H22" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1385,25 +1379,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
       <c r="G23" t="s">
         <v>84</v>
-      </c>
-      <c r="H23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1411,13 +1399,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D24">
         <v>0.01</v>
+      </c>
+      <c r="E24" t="s">
+        <v>106</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
@@ -1431,13 +1422,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D25">
-        <v>0.01</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
         <v>106</v>
@@ -1454,25 +1445,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26">
         <v>100</v>
       </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26">
-        <v>70</v>
-      </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
       </c>
       <c r="G26" t="s">
         <v>84</v>
-      </c>
-      <c r="H26" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1480,25 +1468,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="D27">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
       <c r="G27" t="s">
         <v>84</v>
-      </c>
-      <c r="H27" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1506,19 +1491,25 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.05</v>
+      </c>
+      <c r="E28" t="s">
+        <v>98</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1526,19 +1517,25 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="D29">
-        <v>50</v>
+        <v>0.05</v>
+      </c>
+      <c r="E29" t="s">
+        <v>98</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1546,22 +1543,25 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="D30">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="H30" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1569,22 +1569,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D31">
-        <v>100</v>
-      </c>
-      <c r="E31" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G31" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1592,22 +1592,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="D32">
-        <v>100</v>
-      </c>
-      <c r="E32" t="s">
-        <v>145</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="H32" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1615,22 +1615,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33">
-        <v>100</v>
-      </c>
-      <c r="E33" t="s">
-        <v>145</v>
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="H33" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1638,25 +1638,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
         <v>85</v>
       </c>
-      <c r="E34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" t="s">
-        <v>94</v>
-      </c>
       <c r="H34" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1664,13 +1661,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35">
-        <v>4.0999999999999996</v>
+        <v>85</v>
+      </c>
+      <c r="E35" t="s">
+        <v>97</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
@@ -1687,16 +1687,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>106</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
@@ -1713,22 +1710,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" t="s">
-        <v>43</v>
+        <v>80</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>106</v>
       </c>
       <c r="F37" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="G37" t="s">
         <v>94</v>
       </c>
       <c r="H37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -1736,25 +1736,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>99</v>
+        <v>42</v>
+      </c>
+      <c r="D38" t="s">
+        <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="G38" t="s">
         <v>94</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -1762,25 +1759,22 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D39">
-        <v>5</v>
-      </c>
-      <c r="E39" t="s">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="G39" t="s">
         <v>94</v>
       </c>
       <c r="H39" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -1788,25 +1782,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D40">
-        <v>15</v>
-      </c>
-      <c r="E40" t="s">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="G40" t="s">
         <v>94</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1814,25 +1805,25 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G41" t="s">
         <v>94</v>
       </c>
       <c r="H41" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -1840,22 +1831,25 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D42">
-        <v>0.01</v>
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>99</v>
       </c>
       <c r="F42" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G42" t="s">
         <v>94</v>
       </c>
       <c r="H42" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -1863,25 +1857,25 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G43" t="s">
         <v>94</v>
       </c>
       <c r="H43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -1889,22 +1883,25 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>97</v>
       </c>
       <c r="F44" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="G44" t="s">
         <v>94</v>
       </c>
       <c r="H44" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -1912,22 +1909,22 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>0.01</v>
       </c>
       <c r="F45" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s">
         <v>94</v>
       </c>
       <c r="H45" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -1935,22 +1932,25 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
-      </c>
-      <c r="D46" t="s">
-        <v>132</v>
+        <v>61</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>106</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="G46" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="H46" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
circle shape of substrate grig - eeeegit rm depliney.csv
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E1985E-68AB-41E6-B859-E18C155E9CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F684BB-CB27-49B4-8478-7870F9042EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="143">
   <si>
     <t>filename</t>
   </si>
@@ -61,24 +61,6 @@
     <t>Substrate length, mm</t>
   </si>
   <si>
-    <t>Разрешение по х</t>
-  </si>
-  <si>
-    <t>substrate_x_res</t>
-  </si>
-  <si>
-    <t>Substrate x resolution, 1/mm</t>
-  </si>
-  <si>
-    <t>Разрешение по у</t>
-  </si>
-  <si>
-    <t>substrate_y_res</t>
-  </si>
-  <si>
-    <t>Substrate y resolution, 1/mm</t>
-  </si>
-  <si>
     <t>Число ядер</t>
   </si>
   <si>
@@ -458,6 +440,15 @@
   </si>
   <si>
     <t>оборотов/мин</t>
+  </si>
+  <si>
+    <t>substrate_res</t>
+  </si>
+  <si>
+    <t>Разрешение сектки подложки</t>
+  </si>
+  <si>
+    <t>Число точек на 1 мм</t>
   </si>
 </sst>
 </file>
@@ -827,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,13 +872,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -898,10 +889,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -910,10 +901,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -921,22 +912,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -944,22 +935,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2">
         <v>-105.8</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -967,22 +958,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -999,16 +990,16 @@
         <v>4.46</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1016,25 +1007,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>290</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1042,25 +1033,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>290</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1068,25 +1059,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1094,25 +1085,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1120,22 +1111,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1143,19 +1134,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1163,22 +1154,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D14" s="2">
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F14" t="s">
         <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1192,16 +1183,16 @@
         <v>8</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
         <v>9</v>
@@ -1218,16 +1209,16 @@
         <v>11</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -1238,25 +1229,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1264,10 +1255,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D18">
         <v>0.01</v>
@@ -1276,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1284,22 +1275,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D19">
         <v>0.01</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s">
         <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1307,25 +1298,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D20">
         <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1333,25 +1324,25 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D21">
         <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1359,10 +1350,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1371,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1379,10 +1370,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D23">
         <v>50</v>
@@ -1391,7 +1382,7 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1399,22 +1390,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D24">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1422,22 +1413,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D25">
         <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F25" t="s">
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1445,22 +1436,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D26">
         <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1468,22 +1459,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D27">
         <v>100</v>
       </c>
       <c r="E27" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1491,466 +1482,440 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="D28">
         <v>0.05</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D29">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F29" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H29" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>31</v>
-      </c>
       <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H31" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" t="s">
         <v>19</v>
       </c>
-      <c r="C32" t="s">
+      <c r="G32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" t="s">
         <v>20</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" t="s">
-        <v>85</v>
-      </c>
-      <c r="H32" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" t="s">
         <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" t="s">
-        <v>95</v>
+        <v>72</v>
+      </c>
+      <c r="D34">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>91</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H34" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D35">
-        <v>85</v>
-      </c>
-      <c r="E35" t="s">
-        <v>97</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
       </c>
       <c r="G35" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H35" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D36">
-        <v>4.0999999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>100</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H36" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
-        <v>83</v>
-      </c>
       <c r="C37" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>106</v>
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="G37" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H37" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" t="s">
-        <v>43</v>
+        <v>57</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H38" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>65</v>
-      </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>93</v>
       </c>
       <c r="F40" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H40" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F41" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" t="s">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" t="s">
-        <v>46</v>
-      </c>
       <c r="G42" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H42" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D43">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F43" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G43" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H43" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44">
+        <v>0.01</v>
+      </c>
+      <c r="F44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" t="s">
         <v>53</v>
-      </c>
-      <c r="C44" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" t="s">
-        <v>55</v>
-      </c>
-      <c r="G44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H44" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D45">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>100</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G45" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>60</v>
-      </c>
-      <c r="C46" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>106</v>
-      </c>
-      <c r="F46" t="s">
-        <v>55</v>
-      </c>
-      <c r="G46" t="s">
-        <v>94</v>
-      </c>
-      <c r="H46" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
useful version with multiprocessing pool and thread-memory safety deposition
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420B2C87-304C-41B2-BC2B-1C3489049CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6504FA89-5F97-4CC7-9A61-081B62CE63E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1461,7 +1461,7 @@
         <v>63</v>
       </c>
       <c r="D24">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
log with messages of integrators, adaptive limits of integrators
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569F6048-6C18-4874-BCEE-E3494F1A63B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD0BD20-A00B-49C5-9DB8-3F036CEC61F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="150">
   <si>
     <t>filename</t>
   </si>
@@ -98,15 +98,6 @@
   </si>
   <si>
     <t>needed relative tolerance for thickness in each point</t>
-  </si>
-  <si>
-    <t>Максимальный шаг по углу</t>
-  </si>
-  <si>
-    <t>max_angle_divisions</t>
-  </si>
-  <si>
-    <t>limit of da while integration = 1 degree / max_angle_divisions</t>
   </si>
   <si>
     <t>holder_inner_radius</t>
@@ -848,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -900,19 +891,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
@@ -923,10 +914,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -935,13 +926,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -949,25 +940,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -975,25 +966,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D5" s="2">
         <v>-105.8</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1001,25 +992,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1036,16 +1027,16 @@
         <v>4.46</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1053,25 +1044,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>290</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1079,25 +1070,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>290</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1105,25 +1096,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1131,25 +1122,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1157,22 +1148,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s">
         <v>124</v>
-      </c>
-      <c r="D12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1180,19 +1171,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" t="s">
-        <v>131</v>
-      </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1200,25 +1191,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D14" s="2">
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
         <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1235,16 +1226,16 @@
         <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
         <v>8</v>
@@ -1255,7 +1246,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1264,16 +1255,16 @@
         <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
@@ -1284,25 +1275,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
         <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1310,10 +1301,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
         <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
       </c>
       <c r="D18">
         <v>0.01</v>
@@ -1322,10 +1313,10 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1333,22 +1324,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
         <v>83</v>
-      </c>
-      <c r="C19" t="s">
-        <v>86</v>
       </c>
       <c r="D19">
         <v>0.01</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
         <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1356,19 +1347,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1376,28 +1367,28 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1405,28 +1396,28 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1434,10 +1425,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1446,10 +1437,10 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1457,10 +1448,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1469,10 +1460,10 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1480,22 +1471,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1503,22 +1494,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1526,22 +1517,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D27">
         <v>100</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1549,25 +1540,25 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D28">
         <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1575,25 +1566,25 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D29">
         <v>0.05</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1610,13 +1601,13 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
         <v>25</v>
@@ -1627,22 +1618,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I31" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1650,22 +1641,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I32" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -1673,22 +1664,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
         <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I33" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -1696,22 +1687,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
-        <v>88</v>
+        <v>68</v>
+      </c>
+      <c r="D34">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>87</v>
       </c>
       <c r="F34" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I34" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -1719,25 +1713,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D35">
-        <v>85</v>
-      </c>
-      <c r="E35" t="s">
-        <v>90</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
       </c>
       <c r="G35" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="H35" t="s">
+        <v>143</v>
       </c>
       <c r="I35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -1745,25 +1739,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D36">
-        <v>4.0999999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>96</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>87</v>
-      </c>
-      <c r="H36" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="I36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -1771,25 +1765,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>99</v>
+        <v>32</v>
+      </c>
+      <c r="D37" t="s">
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="G37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -1797,22 +1788,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I38" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -1829,10 +1820,10 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I39" t="s">
         <v>57</v>
@@ -1843,22 +1834,25 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
       </c>
       <c r="F40" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="G40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I40" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -1866,22 +1860,25 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D41">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G41" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="H41" t="s">
+        <v>143</v>
       </c>
       <c r="I41" t="s">
         <v>40</v>
@@ -1898,22 +1895,19 @@
         <v>42</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F42" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G42" t="s">
-        <v>87</v>
-      </c>
-      <c r="H42" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="I42" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -1921,25 +1915,25 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" t="s">
         <v>45</v>
       </c>
-      <c r="D43">
-        <v>15</v>
-      </c>
-      <c r="E43" t="s">
-        <v>92</v>
-      </c>
-      <c r="F43" t="s">
-        <v>39</v>
-      </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I43" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -1947,22 +1941,22 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>90</v>
+        <v>0.01</v>
       </c>
       <c r="F44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="H44" t="s">
+        <v>143</v>
       </c>
       <c r="I44" t="s">
         <v>49</v>
@@ -1979,45 +1973,19 @@
         <v>51</v>
       </c>
       <c r="D45">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>96</v>
       </c>
       <c r="F45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
-      </c>
-      <c r="H45" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="I45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>99</v>
-      </c>
-      <c r="F46" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" t="s">
-        <v>87</v>
-      </c>
-      <c r="I46" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
interface fixes for bsplines using
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5DF9A3-132D-4BC1-BFFB-58C5892EDE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C78E7C-9AE6-490A-A1DF-4B4AF2413C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="142">
   <si>
     <t>Способ задания профиля распыления</t>
   </si>
@@ -313,54 +313,15 @@
     <t>Число точек на 1 мм</t>
   </si>
   <si>
-    <t>Точность в точке</t>
-  </si>
-  <si>
-    <t>point_tolerance</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
     <t>%100</t>
   </si>
   <si>
-    <t>needed relative tolerance for thickness in each point</t>
-  </si>
-  <si>
-    <t>Число ядер</t>
-  </si>
-  <si>
-    <t>cores</t>
-  </si>
-  <si>
     <t>+int</t>
   </si>
   <si>
-    <t>sys</t>
-  </si>
-  <si>
-    <t>number of jobs for paralleling</t>
-  </si>
-  <si>
-    <t>Подробный лог</t>
-  </si>
-  <si>
-    <t>verbose</t>
-  </si>
-  <si>
-    <t>True: print message each time when function of deposition called</t>
-  </si>
-  <si>
-    <t>Стирать кэш</t>
-  </si>
-  <si>
-    <t>delete_cache</t>
-  </si>
-  <si>
-    <t>True: delete history of function evaluations in the beggining of work. Warning: if = False, some changes in the code may be ignored</t>
-  </si>
-  <si>
     <t>Начальное приближение R</t>
   </si>
   <si>
@@ -488,6 +449,15 @@
   </si>
   <si>
     <t>saves\Ns.txt</t>
+  </si>
+  <si>
+    <t>tolerance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точность границ </t>
+  </si>
+  <si>
+    <t>Относительная точность определения углов, при которых траектория точки пересекает узлы сплайна, описывающего профиль. Может влиять на результаты расчёта толщины.</t>
   </si>
 </sst>
 </file>
@@ -516,7 +486,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -539,27 +509,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -864,16 +820,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="2" max="2" width="32.5234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.89453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="254.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -939,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1611,25 +1570,25 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+      <c r="E30" t="s">
         <v>93</v>
       </c>
-      <c r="C30" t="s">
+      <c r="F30" t="s">
         <v>94</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" t="s">
-        <v>96</v>
       </c>
       <c r="G30" t="s">
         <v>91</v>
       </c>
       <c r="I30" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1637,22 +1596,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="G31" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1660,22 +1616,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" t="b">
+        <v>137</v>
+      </c>
+      <c r="D32">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I32" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1683,22 +1636,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" t="b">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="D33">
+        <v>85</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="G33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I33" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1706,25 +1662,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D34">
-        <v>85</v>
-      </c>
-      <c r="E34" t="s">
-        <v>18</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F34" t="s">
         <v>25</v>
       </c>
       <c r="G34" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="H34" t="s">
+        <v>63</v>
       </c>
       <c r="I34" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1732,25 +1688,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D35">
-        <v>4.0999999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
       </c>
       <c r="F35" t="s">
         <v>25</v>
       </c>
       <c r="G35" t="s">
-        <v>111</v>
-      </c>
-      <c r="H35" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="I35" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1758,25 +1714,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>66</v>
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
       </c>
       <c r="F36" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="G36" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="I36" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1784,22 +1737,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
+        <v>98</v>
+      </c>
+      <c r="I37" t="s">
         <v>111</v>
-      </c>
-      <c r="I37" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1807,22 +1760,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G38" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="I38" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1830,22 +1783,25 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="G39" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="I39" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1853,25 +1809,28 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D40">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G40" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="H40" t="s">
+        <v>63</v>
       </c>
       <c r="I40" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1879,28 +1838,25 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G41" t="s">
-        <v>111</v>
-      </c>
-      <c r="H41" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="I41" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1908,25 +1864,25 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D42">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="G42" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="I42" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1934,25 +1890,25 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>18</v>
+        <v>0.01</v>
       </c>
       <c r="F43" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G43" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="H43" t="s">
+        <v>63</v>
       </c>
       <c r="I43" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1960,91 +1916,25 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D44">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
       </c>
       <c r="F44" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G44" t="s">
-        <v>111</v>
-      </c>
-      <c r="H44" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="I44" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>66</v>
-      </c>
-      <c r="F45" t="s">
-        <v>139</v>
-      </c>
-      <c r="G45" t="s">
-        <v>111</v>
-      </c>
-      <c r="I45" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>147</v>
-      </c>
-      <c r="C46" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="2">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>149</v>
-      </c>
-      <c r="C47" t="s">
-        <v>150</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>100</v>
-      </c>
-      <c r="G47" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some fixes with settings
</commit_message>
<xml_diff>
--- a/saves/settings.xlsx
+++ b/saves/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C78E7C-9AE6-490A-A1DF-4B4AF2413C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472CF18C-1C2D-4CCB-8F6D-F954E5FAD8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="144">
   <si>
     <t>Способ задания профиля распыления</t>
   </si>
@@ -448,9 +448,6 @@
     <t>spline_order</t>
   </si>
   <si>
-    <t>saves\Ns.txt</t>
-  </si>
-  <si>
     <t>tolerance</t>
   </si>
   <si>
@@ -458,6 +455,15 @@
   </si>
   <si>
     <t>Относительная точность определения углов, при которых траектория точки пересекает узлы сплайна, описывающего профиль. Может влиять на результаты расчёта толщины.</t>
+  </si>
+  <si>
+    <t>saves/Ns.txt</t>
+  </si>
+  <si>
+    <t>Отладка</t>
+  </si>
+  <si>
+    <t>debug</t>
   </si>
 </sst>
 </file>
@@ -820,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -898,7 +904,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1570,10 +1576,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D30">
         <v>0.1</v>
@@ -1588,7 +1594,7 @@
         <v>91</v>
       </c>
       <c r="I30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1935,6 +1941,26 @@
       </c>
       <c r="I44" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>